<commit_message>
change file name of the source files
</commit_message>
<xml_diff>
--- a/Doc/脸书总结.xlsx
+++ b/Doc/脸书总结.xlsx
@@ -35,19 +35,10 @@
     <t>解法</t>
   </si>
   <si>
-    <t>283. MoveZeros</t>
-  </si>
-  <si>
     <t>Selection Sort</t>
   </si>
   <si>
-    <t>325. Maximum Size Subarray Sum Equals k</t>
-  </si>
-  <si>
     <t>Prefix Sum</t>
-  </si>
-  <si>
-    <t>301. Remove Invalid Parentheses</t>
   </si>
   <si>
     <t>dfs</t>
@@ -57,207 +48,9 @@
 Second sweep deltes possible </t>
   </si>
   <si>
-    <t>67. Add Binary</t>
-  </si>
-  <si>
     <t>String/Array</t>
   </si>
   <si>
-    <t>311. Sparse Matrix Multi</t>
-  </si>
-  <si>
-    <t>273. Integer To English Words</t>
-  </si>
-  <si>
-    <t>17. Letter Combination of a Phone Number</t>
-  </si>
-  <si>
-    <t>278. First Bad Version</t>
-  </si>
-  <si>
-    <t>91. Decode Ways</t>
-  </si>
-  <si>
-    <t>253. Meeting Room II</t>
-  </si>
-  <si>
-    <t>10. Regular Expression Matching</t>
-  </si>
-  <si>
-    <t>15. 3Sum</t>
-  </si>
-  <si>
-    <t>277. Find the Celebrity</t>
-  </si>
-  <si>
-    <t>158. Read N Characters Given Read 4 II - Call multiple times</t>
-  </si>
-  <si>
-    <t>297. Serialize and Deserialize Binary Tree</t>
-  </si>
-  <si>
-    <t>200. Number of Islands</t>
-  </si>
-  <si>
-    <t>282. Expression Add Operatiors</t>
-  </si>
-  <si>
-    <t>76. Minimum Window Substring</t>
-  </si>
-  <si>
-    <t>257. Binary Tree Paths</t>
-  </si>
-  <si>
-    <t>23. Merge k Sorted Lists</t>
-  </si>
-  <si>
-    <t>161. One Edit Distance</t>
-  </si>
-  <si>
-    <t>157. Read N Characters Given Read4</t>
-  </si>
-  <si>
-    <t>285. Inorder Successor in BST</t>
-  </si>
-  <si>
-    <t>121. Best Time to Buy and Sell Stock</t>
-  </si>
-  <si>
-    <t>139. Word Break</t>
-  </si>
-  <si>
-    <t>56. Merge Intervals</t>
-  </si>
-  <si>
-    <t>341. Flatten Nested List Iterator</t>
-  </si>
-  <si>
-    <t>1. Two Sum</t>
-  </si>
-  <si>
-    <t>173. Binary Search Tree Iterator</t>
-  </si>
-  <si>
-    <t>125. Valid Palindrome</t>
-  </si>
-  <si>
-    <t>75. Sort Colors</t>
-  </si>
-  <si>
-    <t>78. Subsets</t>
-  </si>
-  <si>
-    <t>98. Validate Binary Search Tree</t>
-  </si>
-  <si>
-    <t>43. Multiply Strings</t>
-  </si>
-  <si>
-    <t>206. Reverse Linked List</t>
-  </si>
-  <si>
-    <t>133. Clone Graph</t>
-  </si>
-  <si>
-    <t>252. Meeting Rooms</t>
-  </si>
-  <si>
-    <t>218. The Skyline Problem</t>
-  </si>
-  <si>
-    <t>236. Lowest Common Ancestor of a Binary Tree</t>
-  </si>
-  <si>
-    <t>49. Group Anagrams</t>
-  </si>
-  <si>
-    <t>79. Word Search</t>
-  </si>
-  <si>
-    <t>238. Product of Array Except Self</t>
-  </si>
-  <si>
-    <t>38. Count and Say</t>
-  </si>
-  <si>
-    <t>215. Kth Largest Element in an Array</t>
-  </si>
-  <si>
-    <t>209. Minimum Size Subarray Sum</t>
-  </si>
-  <si>
-    <t>57. Insert Interval</t>
-  </si>
-  <si>
-    <t>71. Simplify Path</t>
-  </si>
-  <si>
-    <t>13. Roman to Integer</t>
-  </si>
-  <si>
-    <t>146. LRU Cache</t>
-  </si>
-  <si>
-    <t>33. Search in Rotated Sorted Array</t>
-  </si>
-  <si>
-    <t>208. Implement Trie (Prefix Tree)</t>
-  </si>
-  <si>
-    <t>90. Subsets II</t>
-  </si>
-  <si>
-    <t>44. Wildcard Matching</t>
-  </si>
-  <si>
-    <t>380. Insert Delete GetRandom O(1)</t>
-  </si>
-  <si>
-    <t>128. Longest Consecutive Sequence</t>
-  </si>
-  <si>
-    <t>102. Binary Tree Level Order Traversal</t>
-  </si>
-  <si>
-    <t>377. Combination Sum IV</t>
-  </si>
-  <si>
-    <t>88. Merge Sorted Array</t>
-  </si>
-  <si>
-    <t>28. Implement strStr()</t>
-  </si>
-  <si>
-    <t>334. Incresing Triplet Subsequence</t>
-  </si>
-  <si>
-    <t>494. Target Sum</t>
-  </si>
-  <si>
-    <t>398. Random Pick Index</t>
-  </si>
-  <si>
-    <t>127. Word Ladder</t>
-  </si>
-  <si>
-    <t>50. Pow(x, n)</t>
-  </si>
-  <si>
-    <t>269. Alien Dictionary</t>
-  </si>
-  <si>
-    <t>20. Valid Parentheses</t>
-  </si>
-  <si>
-    <t>235. Lowest Common Ancestor of a Binary Search Tree</t>
-  </si>
-  <si>
-    <t>286. Walls and Gates</t>
-  </si>
-  <si>
-    <t>69. Sqrt(x)</t>
-  </si>
-  <si>
     <t>117. Populating Next Right Pointers in Each Node II</t>
   </si>
   <si>
@@ -346,6 +139,213 @@
   </si>
   <si>
     <t>Heap</t>
+  </si>
+  <si>
+    <t>MoveZeros</t>
+  </si>
+  <si>
+    <t>Maximum Size Subarray Sum Equals k</t>
+  </si>
+  <si>
+    <t>Remove Invalid Parentheses</t>
+  </si>
+  <si>
+    <t>Add Binary</t>
+  </si>
+  <si>
+    <t>Sparse Matrix Multi</t>
+  </si>
+  <si>
+    <t>One Edit Distance</t>
+  </si>
+  <si>
+    <t>Integer To English Words</t>
+  </si>
+  <si>
+    <t>Letter Combination of a Phone Number</t>
+  </si>
+  <si>
+    <t>Number of Islands</t>
+  </si>
+  <si>
+    <t>Expression Add Operatiors</t>
+  </si>
+  <si>
+    <t>Binary Tree Paths</t>
+  </si>
+  <si>
+    <t>First Bad Version</t>
+  </si>
+  <si>
+    <t>Decode Ways</t>
+  </si>
+  <si>
+    <t>Regular Expression Matching</t>
+  </si>
+  <si>
+    <t>Meeting Room II</t>
+  </si>
+  <si>
+    <t>3Sum</t>
+  </si>
+  <si>
+    <t>Find the Celebrity</t>
+  </si>
+  <si>
+    <t>Read N Characters Given Read 4 II - Call multiple times</t>
+  </si>
+  <si>
+    <t>Serialize and Deserialize Binary Tree</t>
+  </si>
+  <si>
+    <t>Minimum Window Substring</t>
+  </si>
+  <si>
+    <t>Merge k Sorted Lists</t>
+  </si>
+  <si>
+    <t>Read N Characters Given Read4</t>
+  </si>
+  <si>
+    <t>Inorder Successor in BST</t>
+  </si>
+  <si>
+    <t>Best Time to Buy and Sell Stock</t>
+  </si>
+  <si>
+    <t>Word Break</t>
+  </si>
+  <si>
+    <t>Merge Intervals</t>
+  </si>
+  <si>
+    <t>Flatten Nested List Iterator</t>
+  </si>
+  <si>
+    <t>Two Sum</t>
+  </si>
+  <si>
+    <t>Binary Search Tree Iterator</t>
+  </si>
+  <si>
+    <t>Valid Palindrome</t>
+  </si>
+  <si>
+    <t>Sort Colors</t>
+  </si>
+  <si>
+    <t>Subsets</t>
+  </si>
+  <si>
+    <t>Validate Binary Search Tree</t>
+  </si>
+  <si>
+    <t>Multiply Strings</t>
+  </si>
+  <si>
+    <t>Reverse Linked List</t>
+  </si>
+  <si>
+    <t>Clone Graph</t>
+  </si>
+  <si>
+    <t>Meeting Rooms</t>
+  </si>
+  <si>
+    <t>The Skyline Problem</t>
+  </si>
+  <si>
+    <t>Lowest Common Ancestor of a Binary Tree</t>
+  </si>
+  <si>
+    <t>Group Anagrams</t>
+  </si>
+  <si>
+    <t>Word Search</t>
+  </si>
+  <si>
+    <t>Product of Array Except Self</t>
+  </si>
+  <si>
+    <t>Count and Say</t>
+  </si>
+  <si>
+    <t>Kth Largest Element in an Array</t>
+  </si>
+  <si>
+    <t>Minimum Size Subarray Sum</t>
+  </si>
+  <si>
+    <t>Insert Interval</t>
+  </si>
+  <si>
+    <t>Simplify Path</t>
+  </si>
+  <si>
+    <t>Roman to Integer</t>
+  </si>
+  <si>
+    <t>LRU Cache</t>
+  </si>
+  <si>
+    <t>Search in Rotated Sorted Array</t>
+  </si>
+  <si>
+    <t>Implement Trie (Prefix Tree)</t>
+  </si>
+  <si>
+    <t>Subsets II</t>
+  </si>
+  <si>
+    <t>Wildcard Matching</t>
+  </si>
+  <si>
+    <t>Insert Delete GetRandom O(1)</t>
+  </si>
+  <si>
+    <t>Longest Consecutive Sequence</t>
+  </si>
+  <si>
+    <t>Binary Tree Level Order Traversal</t>
+  </si>
+  <si>
+    <t>Combination Sum IV</t>
+  </si>
+  <si>
+    <t>Merge Sorted Array</t>
+  </si>
+  <si>
+    <t>Implement strStr()</t>
+  </si>
+  <si>
+    <t>Incresing Triplet Subsequence</t>
+  </si>
+  <si>
+    <t>Target Sum</t>
+  </si>
+  <si>
+    <t>Random Pick Index</t>
+  </si>
+  <si>
+    <t>Word Ladder</t>
+  </si>
+  <si>
+    <t>Pow(x, n)</t>
+  </si>
+  <si>
+    <t>Alien Dictionary</t>
+  </si>
+  <si>
+    <t>Valid Parentheses</t>
+  </si>
+  <si>
+    <t>Lowest Common Ancestor of a Binary Search Tree</t>
+  </si>
+  <si>
+    <t>Walls and Gates</t>
+  </si>
+  <si>
+    <t>Sqrt(x)</t>
   </si>
 </sst>
 </file>
@@ -674,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,495 +698,495 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>99</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>100</v>
+        <v>31</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>101</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>102</v>
+        <v>33</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>103</v>
+        <v>34</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>104</v>
+        <v>35</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>105</v>
+        <v>36</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>106</v>
+        <v>37</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" s="2" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" s="2" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" s="2" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" s="2" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" s="2" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" s="2" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B48" s="2" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49" s="2" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B50" s="2" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B51" s="2" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B52" s="2" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B53" s="2" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B54" s="2" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B55" s="2" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B56" s="2" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B57" s="2" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B58" s="2" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B59" s="2" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B60" s="2" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B61" s="2" t="s">
-        <v>67</v>
+        <v>97</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B62" s="2" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B63" s="2" t="s">
-        <v>69</v>
+        <v>99</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B64" s="2" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65" s="2" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66" s="2" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B67" s="2" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B68" s="2" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B69" s="2" t="s">
-        <v>75</v>
+        <v>105</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B70" s="2" t="s">
-        <v>76</v>
+        <v>106</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B71" s="2" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B72" s="2" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B73" s="2" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B74" s="2" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B75" s="2" t="s">
-        <v>81</v>
+        <v>12</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B76" s="2" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B77" s="2" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B78" s="2" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B79" s="2" t="s">
-        <v>85</v>
+        <v>16</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B80" s="2" t="s">
-        <v>86</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B81" s="2" t="s">
-        <v>87</v>
+        <v>18</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B82" s="2" t="s">
-        <v>88</v>
+        <v>19</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B83" s="2" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B84" s="2" t="s">
-        <v>90</v>
+        <v>21</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B85" s="2" t="s">
-        <v>91</v>
+        <v>22</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B86" s="2" t="s">
-        <v>92</v>
+        <v>23</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B87" s="2" t="s">
-        <v>93</v>
+        <v>24</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B88" s="2" t="s">
-        <v>94</v>
+        <v>25</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B89" s="2" t="s">
-        <v>95</v>
+        <v>26</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B90" s="2" t="s">
-        <v>96</v>
+        <v>27</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B91" s="2" t="s">
-        <v>97</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit range sum + diagonal traverse + find k pairs with smallest sum + minimal height tree + number of connected components in undirected graph + super ugly number
</commit_message>
<xml_diff>
--- a/Doc/脸书总结.xlsx
+++ b/Doc/脸书总结.xlsx
@@ -51,69 +51,6 @@
     <t>String/Array</t>
   </si>
   <si>
-    <t>117. Populating Next Right Pointers in Each Node II</t>
-  </si>
-  <si>
-    <t>68. Text Justification</t>
-  </si>
-  <si>
-    <t>221. Maximal Square</t>
-  </si>
-  <si>
-    <t>274. H-Index</t>
-  </si>
-  <si>
-    <t>85. Maximal Rectangle</t>
-  </si>
-  <si>
-    <t>210. Course Schedule II</t>
-  </si>
-  <si>
-    <t>25. Reverse Nodes in k-Group</t>
-  </si>
-  <si>
-    <t>234. Palindrom Linked List</t>
-  </si>
-  <si>
-    <t>621. Task Scheduler</t>
-  </si>
-  <si>
-    <t>572. Subtree of Another Tree</t>
-  </si>
-  <si>
-    <t>554. Brick Wall</t>
-  </si>
-  <si>
-    <t>543. Diameter of Binary Tree</t>
-  </si>
-  <si>
-    <t>525. Contiguous Array</t>
-  </si>
-  <si>
-    <t>523. Continuous Subarray Sum</t>
-  </si>
-  <si>
-    <t>477. Total Hamming Distance</t>
-  </si>
-  <si>
-    <t>461. Hamming Distance</t>
-  </si>
-  <si>
-    <t>404. Sum of Left Leaves</t>
-  </si>
-  <si>
-    <t>275. H-index II</t>
-  </si>
-  <si>
-    <t>261. Graph Valid Tree</t>
-  </si>
-  <si>
-    <t>80. Remove Duplicates from Sorted Array II</t>
-  </si>
-  <si>
-    <t>26. Remove Duplicates from Sorted Array</t>
-  </si>
-  <si>
     <t>Encode/Decode</t>
   </si>
   <si>
@@ -346,6 +283,69 @@
   </si>
   <si>
     <t>Sqrt(x)</t>
+  </si>
+  <si>
+    <t>Populating Next Right Pointers in Each Node II</t>
+  </si>
+  <si>
+    <t>Text Justification</t>
+  </si>
+  <si>
+    <t>Maximal Square</t>
+  </si>
+  <si>
+    <t>H-Index</t>
+  </si>
+  <si>
+    <t>Maximal Rectangle</t>
+  </si>
+  <si>
+    <t>Course Schedule II</t>
+  </si>
+  <si>
+    <t>Reverse Nodes in k-Group</t>
+  </si>
+  <si>
+    <t>Palindrom Linked List</t>
+  </si>
+  <si>
+    <t>Task Scheduler</t>
+  </si>
+  <si>
+    <t>Subtree of Another Tree</t>
+  </si>
+  <si>
+    <t>Brick Wall</t>
+  </si>
+  <si>
+    <t>Diameter of Binary Tree</t>
+  </si>
+  <si>
+    <t>Contiguous Array</t>
+  </si>
+  <si>
+    <t>Continuous Subarray Sum</t>
+  </si>
+  <si>
+    <t>Total Hamming Distance</t>
+  </si>
+  <si>
+    <t>Hamming Distance</t>
+  </si>
+  <si>
+    <t>Sum of Left Leaves</t>
+  </si>
+  <si>
+    <t>H-index II</t>
+  </si>
+  <si>
+    <t>Graph Valid Tree</t>
+  </si>
+  <si>
+    <t>Remove Duplicates from Sorted Array II</t>
+  </si>
+  <si>
+    <t>Remove Duplicates from Sorted Array</t>
   </si>
 </sst>
 </file>
@@ -674,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -701,7 +701,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -709,7 +709,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -717,7 +717,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
@@ -728,465 +728,465 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="2" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" s="2" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" s="2" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" s="2" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" s="2" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" s="2" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" s="2" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" s="2" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" s="2" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B48" s="2" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49" s="2" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B50" s="2" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B51" s="2" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B52" s="2" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B53" s="2" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B54" s="2" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B55" s="2" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B56" s="2" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B57" s="2" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B58" s="2" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B59" s="2" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B60" s="2" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B61" s="2" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B62" s="2" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B63" s="2" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B64" s="2" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65" s="2" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66" s="2" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B67" s="2" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B68" s="2" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B69" s="2" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B70" s="2" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B71" s="2" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B72" s="2" t="s">
-        <v>9</v>
+        <v>87</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B73" s="2" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B74" s="2" t="s">
-        <v>11</v>
+        <v>89</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B75" s="2" t="s">
-        <v>12</v>
+        <v>90</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B76" s="2" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B77" s="2" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B78" s="2" t="s">
-        <v>15</v>
+        <v>93</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B79" s="2" t="s">
-        <v>16</v>
+        <v>94</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B80" s="2" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B81" s="2" t="s">
-        <v>18</v>
+        <v>96</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B82" s="2" t="s">
-        <v>19</v>
+        <v>97</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B83" s="2" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B84" s="2" t="s">
-        <v>21</v>
+        <v>99</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B85" s="2" t="s">
-        <v>22</v>
+        <v>100</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B86" s="2" t="s">
-        <v>23</v>
+        <v>101</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B87" s="2" t="s">
-        <v>24</v>
+        <v>102</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B88" s="2" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B89" s="2" t="s">
-        <v>26</v>
+        <v>104</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B90" s="2" t="s">
-        <v>27</v>
+        <v>105</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B91" s="2" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit lonely pixel + longest common prefix + maximum subarray sum equals k + minimum absolute difference in BST + power of 3 + remove element + sparse matrix multiplication + verify preorder serialization of binary tree
</commit_message>
<xml_diff>
--- a/Doc/脸书总结.xlsx
+++ b/Doc/脸书总结.xlsx
@@ -78,9 +78,6 @@
     <t>Heap</t>
   </si>
   <si>
-    <t>MoveZeros</t>
-  </si>
-  <si>
     <t>Maximum Size Subarray Sum Equals k</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>Add Binary</t>
   </si>
   <si>
-    <t>Sparse Matrix Multi</t>
-  </si>
-  <si>
     <t>One Edit Distance</t>
   </si>
   <si>
@@ -346,6 +340,12 @@
   </si>
   <si>
     <t>Remove Duplicates from Sorted Array</t>
+  </si>
+  <si>
+    <t>Move Zeros</t>
+  </si>
+  <si>
+    <t>Sparse Matrix Multiply</t>
   </si>
 </sst>
 </file>
@@ -674,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -701,7 +701,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -709,7 +709,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -717,7 +717,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
@@ -728,18 +728,18 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -747,7 +747,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -755,22 +755,22 @@
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -778,7 +778,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -786,12 +786,12 @@
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -799,7 +799,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -807,17 +807,17 @@
         <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -825,7 +825,7 @@
         <v>14</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -833,7 +833,7 @@
         <v>15</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -841,352 +841,352 @@
         <v>16</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B48" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B50" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B51" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B52" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B53" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B54" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B55" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B56" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B57" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B58" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B59" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B60" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B61" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B62" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B63" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B64" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B67" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B68" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B69" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B70" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B71" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B72" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B73" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B74" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B75" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B76" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B77" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B78" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B79" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B80" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B81" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B82" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B83" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B84" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B85" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B86" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B87" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B88" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B89" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B90" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B91" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>